<commit_message>
More test examples and slides
</commit_message>
<xml_diff>
--- a/scaling-the-monolith-2019/docs/load-tests.xlsx
+++ b/scaling-the-monolith-2019/docs/load-tests.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\r\DanielLarsenNZ\talks\scaling-the-monolith-2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\r\DanielLarsenNZ\talks\scaling-the-monolith-2019\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D42C0E-078E-47B9-98C0-60F333A8D3F7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F5C374-C805-4B9C-9A95-50BE2D1D1E2B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16900" windowHeight="6740" xr2:uid="{867D9BA9-89AC-4FA6-AABE-5922BF8C45DF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16900" windowHeight="6740" activeTab="1" xr2:uid="{867D9BA9-89AC-4FA6-AABE-5922BF8C45DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>Run #</t>
   </si>
@@ -178,6 +179,12 @@
   </si>
   <si>
     <t>50:1</t>
+  </si>
+  <si>
+    <t>EXAMPLE</t>
+  </si>
+  <si>
+    <t>1 x Standard1 App Service</t>
   </si>
 </sst>
 </file>
@@ -577,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F275CEB-2803-4FD6-97FC-9A06BA3B0DAF}">
   <dimension ref="B2:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1527,4 +1534,274 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A5A7A2-9412-4931-8C55-79D65CC8C315}">
+  <dimension ref="B2:T10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.36328125" style="5" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="5.26953125" style="5" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6328125" style="5" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7265625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="9"/>
+      <c r="N2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="3"/>
+      <c r="T2" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="5">
+        <v>100</v>
+      </c>
+      <c r="F4" s="5">
+        <v>361</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5">
+        <v>14386</v>
+      </c>
+      <c r="K4" s="5">
+        <f>H4/60</f>
+        <v>239.76666666666668</v>
+      </c>
+      <c r="N4" s="5">
+        <v>49</v>
+      </c>
+      <c r="P4">
+        <v>3980</v>
+      </c>
+      <c r="Q4">
+        <v>5290</v>
+      </c>
+      <c r="R4" s="6" t="str">
+        <f>"1:"&amp;TEXT(Q4/P4, "#.#")</f>
+        <v>1:1.3</v>
+      </c>
+      <c r="T4" s="8">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="5">
+        <v>100</v>
+      </c>
+      <c r="F5" s="5">
+        <v>361.3</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" ref="G5:G7" si="0">(F4-F5)/F4</f>
+        <v>-8.3102493074795395E-4</v>
+      </c>
+      <c r="H5" s="5">
+        <v>14386</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="5">
+        <f>H5/60</f>
+        <v>239.76666666666668</v>
+      </c>
+      <c r="M5" s="4">
+        <f>-((K4-K5)/K4)</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="5">
+        <v>49</v>
+      </c>
+      <c r="O5" s="4">
+        <f>-((N4-N5)/N4)</f>
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>3980</v>
+      </c>
+      <c r="Q5">
+        <v>5290</v>
+      </c>
+      <c r="R5" s="6" t="str">
+        <f>"1:"&amp;TEXT(Q5/P5, "#.#")</f>
+        <v>1:1.3</v>
+      </c>
+      <c r="S5" s="4"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="5">
+        <v>100</v>
+      </c>
+      <c r="F6" s="5">
+        <v>124.2</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.65624135067810685</v>
+      </c>
+      <c r="H6" s="5">
+        <v>22376</v>
+      </c>
+      <c r="K6" s="5">
+        <f>H6/60</f>
+        <v>372.93333333333334</v>
+      </c>
+      <c r="M6" s="4">
+        <f>-((K5-K6)/K5)</f>
+        <v>0.55540108438759894</v>
+      </c>
+      <c r="N6" s="5">
+        <v>73</v>
+      </c>
+      <c r="O6" s="4">
+        <f>-((N5-N6)/N5)</f>
+        <v>0.48979591836734693</v>
+      </c>
+      <c r="P6">
+        <v>6000</v>
+      </c>
+      <c r="Q6">
+        <v>31</v>
+      </c>
+      <c r="R6" s="6" t="str">
+        <f>TEXT(P6/Q6, "#")&amp;":1"</f>
+        <v>194:1</v>
+      </c>
+      <c r="S6" s="4"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="5">
+        <v>100</v>
+      </c>
+      <c r="F7" s="5">
+        <v>41.8</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.66344605475040264</v>
+      </c>
+      <c r="H7" s="5">
+        <v>23743</v>
+      </c>
+      <c r="K7" s="5">
+        <f>H7/60</f>
+        <v>395.71666666666664</v>
+      </c>
+      <c r="M7" s="4">
+        <f>-((K6-K7)/K6)</f>
+        <v>6.1092241687522267E-2</v>
+      </c>
+      <c r="N7" s="5">
+        <v>87.4</v>
+      </c>
+      <c r="O7" s="4">
+        <f>-((N6-N7)/N6)</f>
+        <v>0.19726027397260282</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="G8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="G9" s="4"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="G10" s="4"/>
+      <c r="M10" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>